<commit_message>
Synced allocation algorythm with code
</commit_message>
<xml_diff>
--- a/Subjects/subject 1/audio_data.xlsx
+++ b/Subjects/subject 1/audio_data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\omer\Documents\GitHub\stp-project\Subjects\subject 1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Documents\GitHub\stp-project\Subjects\subject 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00562E04-CD64-49D6-BE1C-A24D836E60A7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F9177F1-FD94-4898-BB0E-9C6D3DF04D49}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="-4710" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Excel 40 sent" sheetId="1" r:id="rId1"/>
@@ -571,8 +571,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
-      <selection activeCell="I61" sqref="I61"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B62" sqref="B62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1809,7 +1809,7 @@
         <v>61</v>
       </c>
       <c r="B62" s="1">
-        <v>100</v>
+        <v>140</v>
       </c>
       <c r="C62" s="1" t="s">
         <v>30</v>

</xml_diff>